<commit_message>
Update timetable, student groups, and exit handling
Timetable and student CSV files updated to reflect new session and group assignments. UserInterface now calls System.exit(0) after main menu loop for proper termination. No functional changes to admin menu or session management logic.
</commit_message>
<xml_diff>
--- a/CS4013ProjectTeamContributions (1) (1).xlsx
+++ b/CS4013ProjectTeamContributions (1) (1).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29523"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ulcampus-my.sharepoint.com/personal/michael_english_ul_ie/Documents/onedrive/CS4013/202425/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\GitHub\OOD-Project-updated\OOD-GROUP19\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="8_{CAAB5438-3840-42CA-BE66-9B8C4814697E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6DEBDF6-99F3-44D0-AC4A-E3244F76A6EB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CBC4346-2D65-4C9E-9DB5-18D218C2E8B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -258,7 +258,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -368,9 +368,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -408,7 +408,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -514,7 +514,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -656,7 +656,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -667,10 +667,10 @@
   <dimension ref="A1:F56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
@@ -680,7 +680,7 @@
     <col min="6" max="6" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -690,7 +690,7 @@
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75">
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="8" t="s">
@@ -700,7 +700,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75">
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -720,7 +720,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>24416304</v>
       </c>
@@ -740,7 +740,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>24432555</v>
       </c>
@@ -760,7 +760,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>24428965</v>
       </c>
@@ -780,7 +780,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>24406406</v>
       </c>
@@ -800,7 +800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="3">
         <f>SUM(C4:C7)</f>
         <v>0.99999999999999989</v>
@@ -818,7 +818,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
@@ -835,7 +835,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
@@ -852,7 +852,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -872,7 +872,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -892,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -912,7 +912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -932,7 +932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -952,7 +952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -972,7 +972,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -992,7 +992,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -1112,7 +1112,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -1132,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -1172,15 +1172,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="16.5" customHeight="1">
+    <row r="28" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>34</v>
       </c>
       <c r="B28" s="5">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D28">
         <v>70</v>
@@ -1192,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -1212,7 +1212,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -1272,7 +1272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -1292,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>41</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -1372,22 +1372,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" s="5"/>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="5"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>44</v>
       </c>
@@ -1398,7 +1398,7 @@
       <c r="D41" s="4"/>
       <c r="F41" s="3"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="5" t="s">
         <v>46</v>
@@ -1407,14 +1407,14 @@
       <c r="D42" s="4"/>
       <c r="F42" s="3"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
         <v>47</v>
       </c>
@@ -1423,7 +1423,7 @@
       <c r="D44" s="4"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>48</v>
       </c>
@@ -1438,7 +1438,7 @@
       </c>
       <c r="F45" s="3"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>45727</v>
       </c>
@@ -1453,7 +1453,7 @@
       </c>
       <c r="F46" s="3"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>45758</v>
       </c>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="F47" s="3"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="6">
         <v>45819</v>
       </c>
@@ -1483,7 +1483,7 @@
       </c>
       <c r="F48" s="3"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="6">
         <v>45972</v>
       </c>
@@ -1498,7 +1498,7 @@
       </c>
       <c r="F49" s="3"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -1513,7 +1513,7 @@
       </c>
       <c r="F50" s="3"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -1528,7 +1528,7 @@
       </c>
       <c r="F51" s="3"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>65</v>
       </c>
@@ -1543,7 +1543,7 @@
       </c>
       <c r="F52" s="3"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>68</v>
       </c>
@@ -1558,7 +1558,7 @@
       </c>
       <c r="F53" s="3"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>70</v>
       </c>
@@ -1573,10 +1573,10 @@
       </c>
       <c r="F54" s="3"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F55" s="3"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F56" s="3"/>
     </row>
   </sheetData>

</xml_diff>